<commit_message>
modified:   data_historis/BNB_data_historis.xlsx 	modified:   data_historis/BNB_data_historis.xlsx:Zone.Identifier 	modified:   data_historis/BTC_data_historis.xlsx 	modified:   data_historis/BTC_data_historis.xlsx:Zone.Identifier 	modified:   data_historis/ETH_data_historis.xlsx 	modified:   data_historis/ETH_data_historis.xlsx:Zone.Identifier 	modified:   data_historis/SOL_data_historis.xlsx 	modified:   data_historis/SOL_data_historis.xlsx:Zone.Identifier 	modified:   data_historis/USDT_data_historis.xlsx 	modified:   data_historis/USDT_data_historis.xlsx:Zone.Identifier
</commit_message>
<xml_diff>
--- a/data_historis/BNB_data_historis.xlsx
+++ b/data_historis/BNB_data_historis.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1953"/>
+  <dimension ref="A1:L1960"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -90286,6 +90286,328 @@
         </is>
       </c>
     </row>
+    <row r="1954">
+      <c r="A1954" s="1" t="n">
+        <v>1952</v>
+      </c>
+      <c r="B1954" s="2" t="n">
+        <v>45418</v>
+      </c>
+      <c r="C1954" t="n">
+        <v>592.14</v>
+      </c>
+      <c r="D1954" t="n">
+        <v>601.89</v>
+      </c>
+      <c r="E1954" t="n">
+        <v>583.37</v>
+      </c>
+      <c r="F1954" t="n">
+        <v>588.48</v>
+      </c>
+      <c r="G1954" t="n">
+        <v>1522319998</v>
+      </c>
+      <c r="H1954" t="n">
+        <v>86851577038</v>
+      </c>
+      <c r="I1954" t="inlineStr">
+        <is>
+          <t>2024-05-06T00:00:00.000Z</t>
+        </is>
+      </c>
+      <c r="J1954" t="inlineStr">
+        <is>
+          <t>2024-05-06T08:47:00.000Z</t>
+        </is>
+      </c>
+      <c r="K1954" t="inlineStr">
+        <is>
+          <t>2024-05-06T15:11:00.000Z</t>
+        </is>
+      </c>
+      <c r="L1954" t="inlineStr">
+        <is>
+          <t>2024-05-06T23:59:59.999Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1955">
+      <c r="A1955" s="1" t="n">
+        <v>1953</v>
+      </c>
+      <c r="B1955" s="2" t="n">
+        <v>45419</v>
+      </c>
+      <c r="C1955" t="n">
+        <v>588.48</v>
+      </c>
+      <c r="D1955" t="n">
+        <v>599.9400000000001</v>
+      </c>
+      <c r="E1955" t="n">
+        <v>576.72</v>
+      </c>
+      <c r="F1955" t="n">
+        <v>577.49</v>
+      </c>
+      <c r="G1955" t="n">
+        <v>1535678414</v>
+      </c>
+      <c r="H1955" t="n">
+        <v>85229585063</v>
+      </c>
+      <c r="I1955" t="inlineStr">
+        <is>
+          <t>2024-05-07T00:00:00.000Z</t>
+        </is>
+      </c>
+      <c r="J1955" t="inlineStr">
+        <is>
+          <t>2024-05-07T11:19:00.000Z</t>
+        </is>
+      </c>
+      <c r="K1955" t="inlineStr">
+        <is>
+          <t>2024-05-07T23:13:00.000Z</t>
+        </is>
+      </c>
+      <c r="L1955" t="inlineStr">
+        <is>
+          <t>2024-05-07T23:59:59.999Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1956">
+      <c r="A1956" s="1" t="n">
+        <v>1954</v>
+      </c>
+      <c r="B1956" s="2" t="n">
+        <v>45420</v>
+      </c>
+      <c r="C1956" t="n">
+        <v>577.49</v>
+      </c>
+      <c r="D1956" t="n">
+        <v>589.5700000000001</v>
+      </c>
+      <c r="E1956" t="n">
+        <v>575.15</v>
+      </c>
+      <c r="F1956" t="n">
+        <v>588.2</v>
+      </c>
+      <c r="G1956" t="n">
+        <v>1603241013</v>
+      </c>
+      <c r="H1956" t="n">
+        <v>86810379871</v>
+      </c>
+      <c r="I1956" t="inlineStr">
+        <is>
+          <t>2024-05-08T00:00:00.000Z</t>
+        </is>
+      </c>
+      <c r="J1956" t="inlineStr">
+        <is>
+          <t>2024-05-08T22:32:00.000Z</t>
+        </is>
+      </c>
+      <c r="K1956" t="inlineStr">
+        <is>
+          <t>2024-05-08T00:34:00.000Z</t>
+        </is>
+      </c>
+      <c r="L1956" t="inlineStr">
+        <is>
+          <t>2024-05-08T23:59:59.999Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1957">
+      <c r="A1957" s="1" t="n">
+        <v>1955</v>
+      </c>
+      <c r="B1957" s="2" t="n">
+        <v>45421</v>
+      </c>
+      <c r="C1957" t="n">
+        <v>588.2</v>
+      </c>
+      <c r="D1957" t="n">
+        <v>602.59</v>
+      </c>
+      <c r="E1957" t="n">
+        <v>586.73</v>
+      </c>
+      <c r="F1957" t="n">
+        <v>596.03</v>
+      </c>
+      <c r="G1957" t="n">
+        <v>1897318659</v>
+      </c>
+      <c r="H1957" t="n">
+        <v>87965965033</v>
+      </c>
+      <c r="I1957" t="inlineStr">
+        <is>
+          <t>2024-05-09T00:00:00.000Z</t>
+        </is>
+      </c>
+      <c r="J1957" t="inlineStr">
+        <is>
+          <t>2024-05-09T15:28:00.000Z</t>
+        </is>
+      </c>
+      <c r="K1957" t="inlineStr">
+        <is>
+          <t>2024-05-09T01:34:00.000Z</t>
+        </is>
+      </c>
+      <c r="L1957" t="inlineStr">
+        <is>
+          <t>2024-05-09T23:59:59.999Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1958">
+      <c r="A1958" s="1" t="n">
+        <v>1956</v>
+      </c>
+      <c r="B1958" s="2" t="n">
+        <v>45422</v>
+      </c>
+      <c r="C1958" t="n">
+        <v>596.03</v>
+      </c>
+      <c r="D1958" t="n">
+        <v>596.58</v>
+      </c>
+      <c r="E1958" t="n">
+        <v>582.05</v>
+      </c>
+      <c r="F1958" t="n">
+        <v>585.62</v>
+      </c>
+      <c r="G1958" t="n">
+        <v>1521708160</v>
+      </c>
+      <c r="H1958" t="n">
+        <v>86430203567</v>
+      </c>
+      <c r="I1958" t="inlineStr">
+        <is>
+          <t>2024-05-10T00:00:00.000Z</t>
+        </is>
+      </c>
+      <c r="J1958" t="inlineStr">
+        <is>
+          <t>2024-05-10T13:55:00.000Z</t>
+        </is>
+      </c>
+      <c r="K1958" t="inlineStr">
+        <is>
+          <t>2024-05-10T17:34:00.000Z</t>
+        </is>
+      </c>
+      <c r="L1958" t="inlineStr">
+        <is>
+          <t>2024-05-10T23:59:59.999Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1959">
+      <c r="A1959" s="1" t="n">
+        <v>1957</v>
+      </c>
+      <c r="B1959" s="2" t="n">
+        <v>45423</v>
+      </c>
+      <c r="C1959" t="n">
+        <v>585.62</v>
+      </c>
+      <c r="D1959" t="n">
+        <v>594.21</v>
+      </c>
+      <c r="E1959" t="n">
+        <v>581.9</v>
+      </c>
+      <c r="F1959" t="n">
+        <v>592.03</v>
+      </c>
+      <c r="G1959" t="n">
+        <v>1333662111</v>
+      </c>
+      <c r="H1959" t="n">
+        <v>87375564249</v>
+      </c>
+      <c r="I1959" t="inlineStr">
+        <is>
+          <t>2024-05-11T00:00:00.000Z</t>
+        </is>
+      </c>
+      <c r="J1959" t="inlineStr">
+        <is>
+          <t>2024-05-11T20:55:00.000Z</t>
+        </is>
+      </c>
+      <c r="K1959" t="inlineStr">
+        <is>
+          <t>2024-05-11T02:08:00.000Z</t>
+        </is>
+      </c>
+      <c r="L1959" t="inlineStr">
+        <is>
+          <t>2024-05-11T23:59:59.999Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1960">
+      <c r="A1960" s="1" t="n">
+        <v>1958</v>
+      </c>
+      <c r="B1960" s="2" t="n">
+        <v>45424</v>
+      </c>
+      <c r="C1960" t="n">
+        <v>592.03</v>
+      </c>
+      <c r="D1960" t="n">
+        <v>599.1799999999999</v>
+      </c>
+      <c r="E1960" t="n">
+        <v>587.8</v>
+      </c>
+      <c r="F1960" t="n">
+        <v>594.42</v>
+      </c>
+      <c r="G1960" t="n">
+        <v>1276671115</v>
+      </c>
+      <c r="H1960" t="n">
+        <v>87729246606</v>
+      </c>
+      <c r="I1960" t="inlineStr">
+        <is>
+          <t>2024-05-12T00:00:00.000Z</t>
+        </is>
+      </c>
+      <c r="J1960" t="inlineStr">
+        <is>
+          <t>2024-05-12T17:49:00.000Z</t>
+        </is>
+      </c>
+      <c r="K1960" t="inlineStr">
+        <is>
+          <t>2024-05-12T08:20:00.000Z</t>
+        </is>
+      </c>
+      <c r="L1960" t="inlineStr">
+        <is>
+          <t>2024-05-12T23:59:59.999Z</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>